<commit_message>
new files added; raw data visualization updated (from histogram to raster plots); figures updated to save to a folder
</commit_message>
<xml_diff>
--- a/Data/SubList_StimType.xlsx
+++ b/Data/SubList_StimType.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallo\OneDrive\Desktop\Cluster Based Permutation Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallo\OneDrive\Desktop\ClusterBasedPermutationTesting\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1A82C95-77A3-4162-8853-3A15B5B5668C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0EC1D7-9F1F-413D-A45C-7F19C862E9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2040" windowWidth="29040" windowHeight="15720" xr2:uid="{23176C6B-10C8-463E-8E4E-1872A4082945}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{23176C6B-10C8-463E-8E4E-1872A4082945}"/>
   </bookViews>
   <sheets>
     <sheet name="SubList_StimType" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>SubID</t>
   </si>
   <si>
-    <t>StimType</t>
-  </si>
-  <si>
     <t>TmazeS01_10Hz_0002_DW_All</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>TmazeS02_iTBS600_024_DW_All</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164CFD1B-A673-4F5E-8D71-DB33596DD02A}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1002,12 +1004,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1015,7 +1017,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1023,7 +1025,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1031,7 +1033,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1039,7 +1041,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1047,7 +1049,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1055,7 +1057,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1063,7 +1065,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1071,7 +1073,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1079,7 +1081,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1087,7 +1089,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1095,7 +1097,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1103,7 +1105,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1111,7 +1113,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1119,7 +1121,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1127,7 +1129,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1135,7 +1137,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1143,7 +1145,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1151,7 +1153,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1159,7 +1161,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1167,7 +1169,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1175,7 +1177,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1183,7 +1185,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1191,7 +1193,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1199,7 +1201,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1207,7 +1209,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1215,7 +1217,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1223,7 +1225,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1231,7 +1233,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1239,7 +1241,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1247,7 +1249,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1255,7 +1257,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1263,7 +1265,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1271,7 +1273,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1</v>

</xml_diff>